<commit_message>
run hierarchical opt fatto
</commit_message>
<xml_diff>
--- a/performance/prestazioni_algoritmi_SNA.xlsx
+++ b/performance/prestazioni_algoritmi_SNA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi\SNA\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7F2417-53A2-4E77-A669-BEE3F38FCBFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F2D32F-DF5D-43DC-9DED-A7A9A8E33158}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="5640" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,26 @@
     <sheet name="EXERCISE 3" sheetId="4" r:id="rId4"/>
     <sheet name="EXERCISE 4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>degree</t>
   </si>
@@ -164,6 +173,24 @@
   </si>
   <si>
     <t>CLOSENESS PARALLEL</t>
+  </si>
+  <si>
+    <t>LANCIO 7</t>
+  </si>
+  <si>
+    <t>LANCIO 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANCIO 9 </t>
+  </si>
+  <si>
+    <t>LANCIO 10</t>
+  </si>
+  <si>
+    <t>Hierarchical OPT (GIGI)</t>
+  </si>
+  <si>
+    <t>COMMENTI</t>
   </si>
 </sst>
 </file>
@@ -617,60 +644,118 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B76A97-71F6-499B-92CA-749854610641}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" customWidth="1"/>
-    <col min="2" max="3" width="33.7265625" customWidth="1"/>
-    <col min="4" max="4" width="26.6328125" customWidth="1"/>
-    <col min="5" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" customWidth="1"/>
-    <col min="7" max="7" width="17.81640625" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" customWidth="1"/>
-    <col min="10" max="10" width="14.7265625" customWidth="1"/>
+    <col min="1" max="2" width="30.7265625" customWidth="1"/>
+    <col min="3" max="4" width="33.7265625" customWidth="1"/>
+    <col min="5" max="5" width="26.6328125" customWidth="1"/>
+    <col min="6" max="6" width="20.7265625" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" customWidth="1"/>
+    <col min="12" max="12" width="17.81640625" customWidth="1"/>
+    <col min="13" max="13" width="13.08984375" customWidth="1"/>
+    <col min="14" max="14" width="18.7265625" customWidth="1"/>
+    <col min="15" max="15" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3">
+        <f>AVERAGE(F3:O3)</f>
+        <v>4.3167762756347603</v>
+      </c>
+      <c r="F3">
+        <v>4.2328977584838796</v>
+      </c>
+      <c r="G3">
+        <v>4.3476593494415203</v>
+      </c>
+      <c r="H3">
+        <v>4.2484049797058097</v>
+      </c>
+      <c r="I3">
+        <v>4.2112441062927202</v>
+      </c>
+      <c r="J3">
+        <v>4.18296027183532</v>
+      </c>
+      <c r="K3">
+        <v>4.5008549690246502</v>
+      </c>
+      <c r="L3">
+        <v>4.2073841094970703</v>
+      </c>
+      <c r="M3">
+        <v>4.4207534790039</v>
+      </c>
+      <c r="N3">
+        <v>4.6460390090942303</v>
+      </c>
+      <c r="O3">
+        <v>4.1695647239684996</v>
       </c>
     </row>
   </sheetData>
@@ -682,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B24B19-4E2D-4BC8-9FF5-83F7AC4D9A21}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -787,9 +872,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -907,15 +995,36 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFE96161-A9F2-4025-BD04-7060C82DC995}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D603AB70-4216-4BA9-BA62-12BC632A56B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81A68092-3375-4F2C-9187-CCBC91DE5362}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -930,28 +1039,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D603AB70-4216-4BA9-BA62-12BC632A56B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFE96161-A9F2-4025-BD04-7060C82DC995}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiunta risultati spectral, nuovi file excel e implementazione performance analysis es2
</commit_message>
<xml_diff>
--- a/performance/prestazioni_algoritmi_SNA.xlsx
+++ b/performance/prestazioni_algoritmi_SNA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi\SNA\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F2D32F-DF5D-43DC-9DED-A7A9A8E33158}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA65AFB-F634-452C-A060-5E7B66DDC077}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="5640" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>degree</t>
   </si>
@@ -154,9 +154,6 @@
     <t xml:space="preserve">BETWEENNESS NAÏVE </t>
   </si>
   <si>
-    <t xml:space="preserve">PAGERANK NAÏVE </t>
-  </si>
-  <si>
     <t xml:space="preserve">HITS NAÏVE </t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t xml:space="preserve">HITS PARALLEL </t>
   </si>
   <si>
-    <t xml:space="preserve">PAGERANK VECTORIZED </t>
-  </si>
-  <si>
     <t>CLOSENESS PARALLEL</t>
   </si>
   <si>
@@ -191,6 +185,36 @@
   </si>
   <si>
     <t>COMMENTI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANCIO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANCIO 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANCIO 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANCIO 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANCIO 7 </t>
+  </si>
+  <si>
+    <t>LANCIO 9</t>
+  </si>
+  <si>
+    <t>PAGERANK NAÏVE TOLLERANZA 1E-6</t>
+  </si>
+  <si>
+    <t>PAGERANK NAÏVE TOLLERANZA 1E-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAGERANK VECTORIZED Tolleranza 1e-6 </t>
+  </si>
+  <si>
+    <t>PAGERANK VECTORIZED Tolleranza 1e-8</t>
   </si>
 </sst>
 </file>
@@ -234,10 +258,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,7 +670,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
         <v>22</v>
@@ -702,26 +725,32 @@
         <v>29</v>
       </c>
       <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>46</v>
-      </c>
-      <c r="N1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>82966.5179359912</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <f>AVERAGE(F3:O3)</f>
@@ -765,10 +794,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B24B19-4E2D-4BC8-9FF5-83F7AC4D9A21}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,9 +805,11 @@
     <col min="1" max="1" width="39.7265625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -788,55 +819,138 @@
       <c r="C1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5">
+        <f>AVERAGE(D5:M5)</f>
+        <v>57.877771925926176</v>
+      </c>
+      <c r="D5">
+        <v>57.1544575691223</v>
+      </c>
+      <c r="E5">
+        <v>57.921657085418701</v>
+      </c>
+      <c r="F5">
+        <v>61.6450967788696</v>
+      </c>
+      <c r="G5">
+        <v>57.5576364994049</v>
+      </c>
+      <c r="H5">
+        <v>56.907742261886597</v>
+      </c>
+      <c r="I5">
+        <v>56.983201742172199</v>
+      </c>
+      <c r="J5">
+        <v>56.932199716567901</v>
+      </c>
+      <c r="K5">
+        <v>57.103562355041497</v>
+      </c>
+      <c r="L5">
+        <v>57.684858083724897</v>
+      </c>
+      <c r="M5">
+        <v>58.887307167053201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10">
+        <v>15.047101974487299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>44</v>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12">
+        <v>303.06279754638598</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13">
+        <v>13.9894342422485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>